<commit_message>
Se incorporan algunos cambios a ejemplos en Python
</commit_message>
<xml_diff>
--- a/Validacion/RW-A20-P10-S38/Documentation/Documentacion Ejemplo MEFI.xlsx
+++ b/Validacion/RW-A20-P10-S38/Documentation/Documentacion Ejemplo MEFI.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Otros ordenadores\Mi portátil\Tesis II\Actual tema\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Ejemplos\Validacion\RW-A20-P10-S38\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Prop Geom y de Materiales" sheetId="1" r:id="rId1"/>
@@ -319,7 +319,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="354">
   <si>
     <t>m</t>
   </si>
@@ -1378,6 +1378,9 @@
   </si>
   <si>
     <t>shear-controlled</t>
+  </si>
+  <si>
+    <t>Moderate aspect ratio</t>
   </si>
 </sst>
 </file>
@@ -2059,7 +2062,7 @@
     <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="249">
+  <cellXfs count="248">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2435,9 +2438,6 @@
     <xf numFmtId="166" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -2486,132 +2486,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -2629,6 +2503,132 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2707,7 +2707,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>714375</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>133492</xdr:rowOff>
+      <xdr:rowOff>133493</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2839,7 +2839,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>724710</xdr:colOff>
       <xdr:row>99</xdr:row>
-      <xdr:rowOff>35339</xdr:rowOff>
+      <xdr:rowOff>35338</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2882,8 +2882,8 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>828006</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>6812</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>189374</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4000,8 +4000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="H1:V73"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="W22" sqref="W22"/>
+    <sheetView tabSelected="1" topLeftCell="L22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4012,7 +4012,7 @@
     <col min="10" max="10" width="28.5703125" style="44" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.85546875" style="44" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="12" style="44" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" style="44" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" style="44" customWidth="1"/>
     <col min="15" max="16" width="11.5703125" style="44"/>
     <col min="17" max="17" width="15.7109375" style="44" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="34.28515625" style="44" customWidth="1"/>
@@ -4024,32 +4024,32 @@
   <sheetData>
     <row r="1" spans="10:21" ht="14.45" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="203" t="s">
+      <c r="J2" s="209" t="s">
         <v>333</v>
       </c>
-      <c r="K2" s="204"/>
-      <c r="L2" s="204"/>
-      <c r="M2" s="204"/>
-      <c r="N2" s="205"/>
-      <c r="Q2" s="203" t="s">
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="211"/>
+      <c r="Q2" s="209" t="s">
         <v>336</v>
       </c>
-      <c r="R2" s="204"/>
-      <c r="S2" s="204"/>
-      <c r="T2" s="204"/>
-      <c r="U2" s="205"/>
+      <c r="R2" s="210"/>
+      <c r="S2" s="210"/>
+      <c r="T2" s="210"/>
+      <c r="U2" s="211"/>
     </row>
     <row r="3" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J3" s="11"/>
-      <c r="K3" s="183"/>
-      <c r="L3" s="183"/>
+      <c r="K3" s="182"/>
+      <c r="L3" s="182"/>
       <c r="M3" s="12" t="s">
         <v>56</v>
       </c>
       <c r="N3" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="Q3" s="209" t="s">
+      <c r="Q3" s="215" t="s">
         <v>3</v>
       </c>
       <c r="R3" s="18" t="s">
@@ -4065,17 +4065,17 @@
       <c r="J4" s="76" t="s">
         <v>332</v>
       </c>
-      <c r="L4" s="182" t="s">
+      <c r="L4" s="181" t="s">
         <v>329</v>
       </c>
       <c r="M4" s="177">
-        <v>2667</v>
-      </c>
-      <c r="N4" s="184">
+        <v>2210</v>
+      </c>
+      <c r="N4" s="183">
         <f>M4/25.4</f>
-        <v>105</v>
-      </c>
-      <c r="Q4" s="210"/>
+        <v>87.00787401574803</v>
+      </c>
+      <c r="Q4" s="216"/>
       <c r="R4" s="1"/>
       <c r="S4" s="166"/>
       <c r="T4" s="2"/>
@@ -4085,17 +4085,17 @@
       <c r="J5" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="L5" s="182" t="s">
+      <c r="L5" s="181" t="s">
         <v>330</v>
       </c>
       <c r="M5" s="177">
         <v>1220</v>
       </c>
-      <c r="N5" s="184">
+      <c r="N5" s="183">
         <f>M5/25.4</f>
         <v>48.031496062992126</v>
       </c>
-      <c r="Q5" s="210"/>
+      <c r="Q5" s="216"/>
       <c r="R5" s="1" t="s">
         <v>5</v>
       </c>
@@ -4107,21 +4107,21 @@
       <c r="J6" s="76" t="s">
         <v>128</v>
       </c>
-      <c r="L6" s="182" t="s">
+      <c r="L6" s="181" t="s">
         <v>1</v>
       </c>
       <c r="M6" s="177">
         <v>152.4</v>
       </c>
-      <c r="N6" s="184">
+      <c r="N6" s="183">
         <f t="shared" ref="N6:N7" si="0">M6/25.4</f>
         <v>6.0000000000000009</v>
       </c>
-      <c r="Q6" s="210"/>
+      <c r="Q6" s="216"/>
       <c r="R6" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="S6" s="198"/>
+      <c r="S6" s="197"/>
       <c r="T6" s="23"/>
       <c r="U6" s="25"/>
     </row>
@@ -4129,24 +4129,24 @@
       <c r="J7" s="76" t="s">
         <v>335</v>
       </c>
-      <c r="L7" s="182" t="s">
+      <c r="L7" s="181" t="s">
         <v>334</v>
       </c>
       <c r="M7" s="177">
         <v>304.8</v>
       </c>
-      <c r="N7" s="184">
+      <c r="N7" s="183">
         <f t="shared" si="0"/>
         <v>12.000000000000002</v>
       </c>
-      <c r="Q7" s="210"/>
+      <c r="Q7" s="216"/>
       <c r="R7" s="23" t="s">
         <v>7</v>
       </c>
       <c r="S7" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="T7" s="189">
+      <c r="T7" s="188">
         <v>469.93</v>
       </c>
       <c r="U7" s="25" t="s">
@@ -4154,21 +4154,21 @@
       </c>
     </row>
     <row r="8" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J8" s="185" t="s">
+      <c r="J8" s="184" t="s">
         <v>339</v>
       </c>
-      <c r="K8" s="186"/>
-      <c r="L8" s="196" t="s">
+      <c r="K8" s="185"/>
+      <c r="L8" s="195" t="s">
         <v>340</v>
       </c>
-      <c r="M8" s="197">
+      <c r="M8" s="196">
         <v>228.6</v>
       </c>
-      <c r="N8" s="187">
+      <c r="N8" s="186">
         <f>M8/25.4</f>
         <v>9</v>
       </c>
-      <c r="Q8" s="210"/>
+      <c r="Q8" s="216"/>
       <c r="R8" s="23" t="s">
         <v>10</v>
       </c>
@@ -4178,11 +4178,22 @@
       <c r="T8" s="28"/>
       <c r="U8" s="25"/>
     </row>
-    <row r="9" spans="10:21" x14ac:dyDescent="0.25">
-      <c r="L9" s="182"/>
-      <c r="M9" s="177"/>
-      <c r="N9" s="181"/>
-      <c r="Q9" s="210"/>
+    <row r="9" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="184" t="s">
+        <v>350</v>
+      </c>
+      <c r="K9" s="185"/>
+      <c r="L9" s="195" t="s">
+        <v>351</v>
+      </c>
+      <c r="M9" s="202">
+        <f>M4/M5</f>
+        <v>1.8114754098360655</v>
+      </c>
+      <c r="N9" s="203" t="s">
+        <v>353</v>
+      </c>
+      <c r="Q9" s="216"/>
       <c r="R9" s="3" t="s">
         <v>11</v>
       </c>
@@ -4195,7 +4206,7 @@
       <c r="U9" s="29"/>
     </row>
     <row r="10" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q10" s="210"/>
+      <c r="Q10" s="216"/>
       <c r="R10" s="6" t="s">
         <v>13</v>
       </c>
@@ -4204,18 +4215,18 @@
       <c r="U10" s="30"/>
     </row>
     <row r="11" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J11" s="206" t="s">
+      <c r="J11" s="212" t="s">
         <v>80</v>
       </c>
-      <c r="K11" s="207"/>
-      <c r="L11" s="207"/>
-      <c r="M11" s="207"/>
-      <c r="N11" s="208"/>
-      <c r="Q11" s="210"/>
+      <c r="K11" s="213"/>
+      <c r="L11" s="213"/>
+      <c r="M11" s="213"/>
+      <c r="N11" s="214"/>
+      <c r="Q11" s="216"/>
       <c r="R11" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="S11" s="188"/>
+      <c r="S11" s="187"/>
       <c r="T11" s="23"/>
       <c r="U11" s="25"/>
     </row>
@@ -4235,14 +4246,14 @@
       <c r="N12" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="Q12" s="210"/>
+      <c r="Q12" s="216"/>
       <c r="R12" s="23" t="s">
         <v>7</v>
       </c>
       <c r="S12" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="T12" s="189">
+      <c r="T12" s="188">
         <v>409.71</v>
       </c>
       <c r="U12" s="25" t="s">
@@ -4267,7 +4278,7 @@
         <f>M13/25.4</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="210"/>
+      <c r="Q13" s="216"/>
       <c r="R13" s="23" t="s">
         <v>10</v>
       </c>
@@ -4295,7 +4306,7 @@
         <f t="shared" ref="N14:N32" si="2">M14/25.4</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="210"/>
+      <c r="Q14" s="216"/>
       <c r="R14" s="3" t="s">
         <v>11</v>
       </c>
@@ -4326,7 +4337,7 @@
         <v>12.428740157480316</v>
       </c>
       <c r="O15" s="178"/>
-      <c r="Q15" s="210"/>
+      <c r="Q15" s="216"/>
       <c r="R15" s="6" t="s">
         <v>16</v>
       </c>
@@ -4352,11 +4363,11 @@
         <f t="shared" si="2"/>
         <v>12.428740157480316</v>
       </c>
-      <c r="Q16" s="210"/>
+      <c r="Q16" s="216"/>
       <c r="R16" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="S16" s="188"/>
+      <c r="S16" s="187"/>
       <c r="T16" s="23"/>
       <c r="U16" s="25"/>
     </row>
@@ -4379,14 +4390,14 @@
         <v>24.85708661417323</v>
       </c>
       <c r="O17" s="178"/>
-      <c r="Q17" s="210"/>
+      <c r="Q17" s="216"/>
       <c r="R17" s="23" t="s">
         <v>7</v>
       </c>
       <c r="S17" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="T17" s="189">
+      <c r="T17" s="188">
         <v>429.78</v>
       </c>
       <c r="U17" s="25" t="s">
@@ -4411,7 +4422,7 @@
         <f t="shared" si="2"/>
         <v>24.85708661417323</v>
       </c>
-      <c r="Q18" s="210"/>
+      <c r="Q18" s="216"/>
       <c r="R18" s="23" t="s">
         <v>10</v>
       </c>
@@ -4440,7 +4451,7 @@
         <v>37.285826771653547</v>
       </c>
       <c r="O19" s="178"/>
-      <c r="Q19" s="210"/>
+      <c r="Q19" s="216"/>
       <c r="R19" s="3" t="s">
         <v>11</v>
       </c>
@@ -4471,7 +4482,7 @@
         <f t="shared" si="2"/>
         <v>37.285826771653547</v>
       </c>
-      <c r="Q20" s="210"/>
+      <c r="Q20" s="216"/>
       <c r="R20" s="32" t="s">
         <v>19</v>
       </c>
@@ -4504,7 +4515,7 @@
         <v>49.714173228346461</v>
       </c>
       <c r="O21" s="178"/>
-      <c r="Q21" s="210"/>
+      <c r="Q21" s="216"/>
       <c r="R21" s="32" t="s">
         <v>21</v>
       </c>
@@ -4534,7 +4545,7 @@
         <f t="shared" si="2"/>
         <v>49.714173228346461</v>
       </c>
-      <c r="Q22" s="210"/>
+      <c r="Q22" s="216"/>
       <c r="R22" s="32" t="s">
         <v>24</v>
       </c>
@@ -4565,7 +4576,7 @@
         <v>62.14291338582678</v>
       </c>
       <c r="O23" s="178"/>
-      <c r="Q23" s="211"/>
+      <c r="Q23" s="217"/>
       <c r="R23" s="2"/>
       <c r="S23" s="8" t="s">
         <v>26</v>
@@ -4593,7 +4604,7 @@
         <f t="shared" si="2"/>
         <v>62.14291338582678</v>
       </c>
-      <c r="Q24" s="212" t="s">
+      <c r="Q24" s="218" t="s">
         <v>27</v>
       </c>
       <c r="R24" s="1" t="s">
@@ -4624,7 +4635,7 @@
         <v>74.57125984251968</v>
       </c>
       <c r="O25" s="178"/>
-      <c r="Q25" s="210"/>
+      <c r="Q25" s="216"/>
       <c r="R25" s="6" t="s">
         <v>29</v>
       </c>
@@ -4650,7 +4661,7 @@
         <f t="shared" si="2"/>
         <v>74.57125984251968</v>
       </c>
-      <c r="Q26" s="210"/>
+      <c r="Q26" s="216"/>
       <c r="R26" s="23" t="s">
         <v>30</v>
       </c>
@@ -4683,7 +4694,7 @@
         <v>87.000000000000014</v>
       </c>
       <c r="O27" s="178"/>
-      <c r="Q27" s="210"/>
+      <c r="Q27" s="216"/>
       <c r="R27" s="23" t="s">
         <v>32</v>
       </c>
@@ -4713,14 +4724,14 @@
         <f t="shared" si="2"/>
         <v>87.000000000000014</v>
       </c>
-      <c r="Q28" s="210"/>
+      <c r="Q28" s="216"/>
       <c r="R28" s="23" t="s">
         <v>19</v>
       </c>
       <c r="S28" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="T28" s="194">
+      <c r="T28" s="193">
         <f>4700*SQRT(-T26)</f>
         <v>32252.412312879791</v>
       </c>
@@ -4739,7 +4750,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M29" s="199">
+      <c r="M29" s="198">
         <v>2438.4</v>
       </c>
       <c r="N29" s="179">
@@ -4747,14 +4758,14 @@
         <v>96.000000000000014</v>
       </c>
       <c r="O29" s="178"/>
-      <c r="Q29" s="210"/>
+      <c r="Q29" s="216"/>
       <c r="R29" s="23" t="s">
         <v>34</v>
       </c>
       <c r="S29" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="T29" s="193">
+      <c r="T29" s="192">
         <v>1.02</v>
       </c>
       <c r="U29" s="88"/>
@@ -4771,25 +4782,25 @@
         <f t="shared" si="1"/>
         <v>48.031496062992126</v>
       </c>
-      <c r="M30" s="199">
+      <c r="M30" s="198">
         <v>2438.4</v>
       </c>
       <c r="N30" s="179">
         <f t="shared" si="2"/>
         <v>96.000000000000014</v>
       </c>
-      <c r="Q30" s="210"/>
+      <c r="Q30" s="216"/>
       <c r="R30" s="23" t="s">
         <v>36</v>
       </c>
       <c r="S30" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="T30" s="192">
+      <c r="T30" s="191">
         <f>(-T26/5.2-1.9)</f>
         <v>7.1557692307692307</v>
       </c>
-      <c r="U30" s="191"/>
+      <c r="U30" s="190"/>
     </row>
     <row r="31" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J31" s="14">
@@ -4810,7 +4821,7 @@
         <v>105</v>
       </c>
       <c r="O31" s="178"/>
-      <c r="Q31" s="210"/>
+      <c r="Q31" s="216"/>
       <c r="R31" s="6" t="s">
         <v>37</v>
       </c>
@@ -4836,7 +4847,7 @@
         <f t="shared" si="2"/>
         <v>105</v>
       </c>
-      <c r="Q32" s="210"/>
+      <c r="Q32" s="216"/>
       <c r="R32" s="23" t="s">
         <v>38</v>
       </c>
@@ -4851,7 +4862,7 @@
       </c>
     </row>
     <row r="33" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q33" s="210"/>
+      <c r="Q33" s="216"/>
       <c r="R33" s="23" t="s">
         <v>40</v>
       </c>
@@ -4864,14 +4875,14 @@
       <c r="U33" s="25"/>
     </row>
     <row r="34" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q34" s="210"/>
+      <c r="Q34" s="216"/>
       <c r="R34" s="23" t="s">
         <v>42</v>
       </c>
       <c r="S34" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="T34" s="194">
+      <c r="T34" s="193">
         <f>4700*SQRT(-T32)</f>
         <v>34467.378780522318</v>
       </c>
@@ -4880,34 +4891,34 @@
       </c>
     </row>
     <row r="35" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q35" s="210"/>
+      <c r="Q35" s="216"/>
       <c r="R35" s="23" t="s">
         <v>34</v>
       </c>
       <c r="S35" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="T35" s="193">
+      <c r="T35" s="192">
         <v>1.02</v>
       </c>
       <c r="U35" s="25"/>
     </row>
     <row r="36" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q36" s="210"/>
+      <c r="Q36" s="216"/>
       <c r="R36" s="23" t="s">
         <v>36</v>
       </c>
       <c r="S36" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="T36" s="192">
+      <c r="T36" s="191">
         <f>(-T32/5.2-1.9)</f>
         <v>8.4423076923076916</v>
       </c>
-      <c r="U36" s="191"/>
+      <c r="U36" s="190"/>
     </row>
     <row r="37" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q37" s="210"/>
+      <c r="Q37" s="216"/>
       <c r="R37" s="6" t="s">
         <v>44</v>
       </c>
@@ -4916,14 +4927,14 @@
       <c r="U37" s="30"/>
     </row>
     <row r="38" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q38" s="210"/>
+      <c r="Q38" s="216"/>
       <c r="R38" s="23" t="s">
         <v>45</v>
       </c>
       <c r="S38" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="T38" s="190">
+      <c r="T38" s="189">
         <f>0.31*SQRT(-T26)</f>
         <v>2.1272867695729225</v>
       </c>
@@ -4932,7 +4943,7 @@
       </c>
     </row>
     <row r="39" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q39" s="210"/>
+      <c r="Q39" s="216"/>
       <c r="R39" s="23" t="s">
         <v>46</v>
       </c>
@@ -4945,7 +4956,7 @@
       <c r="U39" s="25"/>
     </row>
     <row r="40" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q40" s="210"/>
+      <c r="Q40" s="216"/>
       <c r="R40" s="23" t="s">
         <v>34</v>
       </c>
@@ -4960,7 +4971,7 @@
       </c>
     </row>
     <row r="41" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q41" s="211"/>
+      <c r="Q41" s="217"/>
       <c r="R41" s="23" t="s">
         <v>36</v>
       </c>
@@ -4973,7 +4984,7 @@
       <c r="U41" s="22"/>
     </row>
     <row r="42" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q42" s="213" t="s">
+      <c r="Q42" s="219" t="s">
         <v>50</v>
       </c>
       <c r="R42" s="6" t="s">
@@ -4986,7 +4997,7 @@
       <c r="U42" s="30"/>
     </row>
     <row r="43" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q43" s="201"/>
+      <c r="Q43" s="207"/>
       <c r="R43" s="6" t="s">
         <v>52</v>
       </c>
@@ -4995,7 +5006,7 @@
       <c r="U43" s="30"/>
     </row>
     <row r="44" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q44" s="201"/>
+      <c r="Q44" s="207"/>
       <c r="R44" s="23" t="s">
         <v>53</v>
       </c>
@@ -5006,7 +5017,7 @@
       <c r="U44" s="25"/>
     </row>
     <row r="45" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q45" s="201"/>
+      <c r="Q45" s="207"/>
       <c r="R45" s="23" t="s">
         <v>54</v>
       </c>
@@ -5021,7 +5032,7 @@
       </c>
     </row>
     <row r="46" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q46" s="201"/>
+      <c r="Q46" s="207"/>
       <c r="R46" s="23" t="s">
         <v>57</v>
       </c>
@@ -5036,7 +5047,7 @@
       </c>
     </row>
     <row r="47" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q47" s="201"/>
+      <c r="Q47" s="207"/>
       <c r="R47" s="23" t="s">
         <v>59</v>
       </c>
@@ -5052,7 +5063,7 @@
       </c>
     </row>
     <row r="48" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q48" s="201"/>
+      <c r="Q48" s="207"/>
       <c r="R48" s="23"/>
       <c r="S48" s="26" t="s">
         <v>306</v>
@@ -5064,7 +5075,7 @@
       <c r="U48" s="25"/>
     </row>
     <row r="49" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q49" s="201"/>
+      <c r="Q49" s="207"/>
       <c r="R49" s="23" t="s">
         <v>61</v>
       </c>
@@ -5078,7 +5089,7 @@
       <c r="U49" s="25"/>
     </row>
     <row r="50" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q50" s="201"/>
+      <c r="Q50" s="207"/>
       <c r="R50" s="6" t="s">
         <v>62</v>
       </c>
@@ -5090,7 +5101,7 @@
       <c r="H51" s="15"/>
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
-      <c r="Q51" s="201"/>
+      <c r="Q51" s="207"/>
       <c r="R51" s="23" t="s">
         <v>63</v>
       </c>
@@ -5105,7 +5116,7 @@
       <c r="I52" s="15"/>
       <c r="J52" s="15"/>
       <c r="N52" s="144"/>
-      <c r="Q52" s="201"/>
+      <c r="Q52" s="207"/>
       <c r="R52" s="23" t="s">
         <v>54</v>
       </c>
@@ -5123,7 +5134,7 @@
       <c r="H53" s="15"/>
       <c r="I53" s="15"/>
       <c r="J53" s="15"/>
-      <c r="Q53" s="201"/>
+      <c r="Q53" s="207"/>
       <c r="R53" s="23" t="s">
         <v>64</v>
       </c>
@@ -5139,7 +5150,7 @@
       </c>
     </row>
     <row r="54" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q54" s="201"/>
+      <c r="Q54" s="207"/>
       <c r="R54" s="23" t="s">
         <v>66</v>
       </c>
@@ -5155,7 +5166,7 @@
       </c>
     </row>
     <row r="55" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q55" s="201"/>
+      <c r="Q55" s="207"/>
       <c r="R55" s="23" t="s">
         <v>61</v>
       </c>
@@ -5169,7 +5180,7 @@
       <c r="U55" s="25"/>
     </row>
     <row r="56" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q56" s="201"/>
+      <c r="Q56" s="207"/>
       <c r="R56" s="6" t="s">
         <v>69</v>
       </c>
@@ -5178,7 +5189,7 @@
       <c r="U56" s="30"/>
     </row>
     <row r="57" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q57" s="201"/>
+      <c r="Q57" s="207"/>
       <c r="R57" s="23" t="s">
         <v>70</v>
       </c>
@@ -5189,7 +5200,7 @@
       <c r="U57" s="25"/>
     </row>
     <row r="58" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q58" s="201"/>
+      <c r="Q58" s="207"/>
       <c r="R58" s="23" t="s">
         <v>54</v>
       </c>
@@ -5205,7 +5216,7 @@
       <c r="V58" s="27"/>
     </row>
     <row r="59" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q59" s="201"/>
+      <c r="Q59" s="207"/>
       <c r="R59" s="23" t="s">
         <v>57</v>
       </c>
@@ -5220,7 +5231,7 @@
       </c>
     </row>
     <row r="60" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q60" s="201"/>
+      <c r="Q60" s="207"/>
       <c r="R60" s="23" t="s">
         <v>71</v>
       </c>
@@ -5233,7 +5244,7 @@
       <c r="U60" s="25"/>
     </row>
     <row r="61" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q61" s="201"/>
+      <c r="Q61" s="207"/>
       <c r="R61" s="23" t="s">
         <v>59</v>
       </c>
@@ -5250,7 +5261,7 @@
       <c r="V61" s="37"/>
     </row>
     <row r="62" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q62" s="201"/>
+      <c r="Q62" s="207"/>
       <c r="R62" s="23" t="s">
         <v>61</v>
       </c>
@@ -5262,10 +5273,10 @@
         <v>8.3105763874489758E-3</v>
       </c>
       <c r="U62" s="25"/>
-      <c r="V62" s="195"/>
+      <c r="V62" s="194"/>
     </row>
     <row r="63" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q63" s="201"/>
+      <c r="Q63" s="207"/>
       <c r="R63" s="6" t="s">
         <v>73</v>
       </c>
@@ -5274,7 +5285,7 @@
       <c r="U63" s="30"/>
     </row>
     <row r="64" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q64" s="201"/>
+      <c r="Q64" s="207"/>
       <c r="R64" s="23" t="s">
         <v>74</v>
       </c>
@@ -5289,7 +5300,7 @@
       </c>
     </row>
     <row r="65" spans="17:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q65" s="202"/>
+      <c r="Q65" s="208"/>
       <c r="R65" s="40" t="s">
         <v>77</v>
       </c>
@@ -5304,7 +5315,7 @@
       </c>
     </row>
     <row r="66" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q66" s="200" t="s">
+      <c r="Q66" s="206" t="s">
         <v>346</v>
       </c>
       <c r="R66" s="18" t="s">
@@ -5317,7 +5328,7 @@
       <c r="U66" s="21"/>
     </row>
     <row r="67" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q67" s="201"/>
+      <c r="Q67" s="207"/>
       <c r="R67" s="6" t="s">
         <v>83</v>
       </c>
@@ -5326,7 +5337,7 @@
       <c r="U67" s="30"/>
     </row>
     <row r="68" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q68" s="201"/>
+      <c r="Q68" s="207"/>
       <c r="R68" s="23" t="s">
         <v>81</v>
       </c>
@@ -5339,7 +5350,7 @@
       <c r="U68" s="45"/>
     </row>
     <row r="69" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q69" s="201"/>
+      <c r="Q69" s="207"/>
       <c r="R69" s="2" t="s">
         <v>86</v>
       </c>
@@ -5352,7 +5363,7 @@
       </c>
     </row>
     <row r="70" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q70" s="201"/>
+      <c r="Q70" s="207"/>
       <c r="R70" s="6" t="s">
         <v>84</v>
       </c>
@@ -5361,7 +5372,7 @@
       <c r="U70" s="49"/>
     </row>
     <row r="71" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q71" s="201"/>
+      <c r="Q71" s="207"/>
       <c r="R71" s="23" t="s">
         <v>85</v>
       </c>
@@ -5374,7 +5385,7 @@
       <c r="U71" s="45"/>
     </row>
     <row r="72" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q72" s="201"/>
+      <c r="Q72" s="207"/>
       <c r="R72" s="23" t="s">
         <v>89</v>
       </c>
@@ -5389,7 +5400,7 @@
       </c>
     </row>
     <row r="73" spans="17:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q73" s="202"/>
+      <c r="Q73" s="208"/>
       <c r="R73" s="40"/>
       <c r="S73" s="41" t="s">
         <v>88</v>
@@ -5423,8 +5434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="H1:V73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5447,32 +5458,32 @@
   <sheetData>
     <row r="1" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="203" t="s">
+      <c r="J2" s="209" t="s">
         <v>333</v>
       </c>
-      <c r="K2" s="204"/>
-      <c r="L2" s="204"/>
-      <c r="M2" s="204"/>
-      <c r="N2" s="205"/>
-      <c r="Q2" s="203" t="s">
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="211"/>
+      <c r="Q2" s="209" t="s">
         <v>336</v>
       </c>
-      <c r="R2" s="204"/>
-      <c r="S2" s="204"/>
-      <c r="T2" s="204"/>
-      <c r="U2" s="205"/>
+      <c r="R2" s="210"/>
+      <c r="S2" s="210"/>
+      <c r="T2" s="210"/>
+      <c r="U2" s="211"/>
     </row>
     <row r="3" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J3" s="11"/>
-      <c r="K3" s="183"/>
-      <c r="L3" s="183"/>
+      <c r="K3" s="182"/>
+      <c r="L3" s="182"/>
       <c r="M3" s="12" t="s">
         <v>56</v>
       </c>
       <c r="N3" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="Q3" s="209" t="s">
+      <c r="Q3" s="215" t="s">
         <v>3</v>
       </c>
       <c r="R3" s="18" t="s">
@@ -5488,19 +5499,19 @@
       <c r="J4" s="76" t="s">
         <v>332</v>
       </c>
-      <c r="K4" s="242"/>
-      <c r="L4" s="243" t="s">
+      <c r="K4" s="199"/>
+      <c r="L4" s="200" t="s">
         <v>329</v>
       </c>
-      <c r="M4" s="244">
+      <c r="M4" s="201">
         <f>2667/2</f>
         <v>1333.5</v>
       </c>
-      <c r="N4" s="184">
+      <c r="N4" s="183">
         <f>M4/25.4</f>
         <v>52.5</v>
       </c>
-      <c r="Q4" s="210"/>
+      <c r="Q4" s="216"/>
       <c r="R4" s="1"/>
       <c r="S4" s="166"/>
       <c r="T4" s="2"/>
@@ -5510,18 +5521,18 @@
       <c r="J5" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="K5" s="242"/>
-      <c r="L5" s="243" t="s">
+      <c r="K5" s="199"/>
+      <c r="L5" s="200" t="s">
         <v>330</v>
       </c>
-      <c r="M5" s="244">
+      <c r="M5" s="201">
         <v>1220</v>
       </c>
-      <c r="N5" s="184">
+      <c r="N5" s="183">
         <f>M5/25.4</f>
         <v>48.031496062992126</v>
       </c>
-      <c r="Q5" s="210"/>
+      <c r="Q5" s="216"/>
       <c r="R5" s="1" t="s">
         <v>5</v>
       </c>
@@ -5533,22 +5544,22 @@
       <c r="J6" s="76" t="s">
         <v>128</v>
       </c>
-      <c r="K6" s="242"/>
-      <c r="L6" s="243" t="s">
+      <c r="K6" s="199"/>
+      <c r="L6" s="200" t="s">
         <v>1</v>
       </c>
-      <c r="M6" s="244">
+      <c r="M6" s="201">
         <v>152.4</v>
       </c>
-      <c r="N6" s="184">
+      <c r="N6" s="183">
         <f t="shared" ref="N6:N7" si="0">M6/25.4</f>
         <v>6.0000000000000009</v>
       </c>
-      <c r="Q6" s="210"/>
+      <c r="Q6" s="216"/>
       <c r="R6" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="S6" s="198"/>
+      <c r="S6" s="197"/>
       <c r="T6" s="23"/>
       <c r="U6" s="25"/>
     </row>
@@ -5556,25 +5567,25 @@
       <c r="J7" s="76" t="s">
         <v>335</v>
       </c>
-      <c r="K7" s="242"/>
-      <c r="L7" s="243" t="s">
+      <c r="K7" s="199"/>
+      <c r="L7" s="200" t="s">
         <v>334</v>
       </c>
-      <c r="M7" s="244">
+      <c r="M7" s="201">
         <v>304.8</v>
       </c>
-      <c r="N7" s="184">
+      <c r="N7" s="183">
         <f t="shared" si="0"/>
         <v>12.000000000000002</v>
       </c>
-      <c r="Q7" s="210"/>
+      <c r="Q7" s="216"/>
       <c r="R7" s="23" t="s">
         <v>7</v>
       </c>
       <c r="S7" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="T7" s="189">
+      <c r="T7" s="188">
         <v>469.93</v>
       </c>
       <c r="U7" s="25" t="s">
@@ -5585,18 +5596,18 @@
       <c r="J8" s="76" t="s">
         <v>339</v>
       </c>
-      <c r="K8" s="242"/>
-      <c r="L8" s="243" t="s">
+      <c r="K8" s="199"/>
+      <c r="L8" s="200" t="s">
         <v>340</v>
       </c>
-      <c r="M8" s="244">
+      <c r="M8" s="201">
         <v>228.6</v>
       </c>
-      <c r="N8" s="184">
+      <c r="N8" s="183">
         <f>M8/25.4</f>
         <v>9</v>
       </c>
-      <c r="Q8" s="210"/>
+      <c r="Q8" s="216"/>
       <c r="R8" s="23" t="s">
         <v>10</v>
       </c>
@@ -5607,21 +5618,21 @@
       <c r="U8" s="25"/>
     </row>
     <row r="9" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J9" s="185" t="s">
+      <c r="J9" s="184" t="s">
         <v>350</v>
       </c>
-      <c r="K9" s="186"/>
-      <c r="L9" s="196" t="s">
+      <c r="K9" s="185"/>
+      <c r="L9" s="195" t="s">
         <v>351</v>
       </c>
-      <c r="M9" s="245">
+      <c r="M9" s="202">
         <f>M4/M5</f>
         <v>1.0930327868852459</v>
       </c>
-      <c r="N9" s="246" t="s">
+      <c r="N9" s="203" t="s">
         <v>352</v>
       </c>
-      <c r="Q9" s="210"/>
+      <c r="Q9" s="216"/>
       <c r="R9" s="3" t="s">
         <v>11</v>
       </c>
@@ -5634,7 +5645,7 @@
       <c r="U9" s="29"/>
     </row>
     <row r="10" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q10" s="210"/>
+      <c r="Q10" s="216"/>
       <c r="R10" s="6" t="s">
         <v>13</v>
       </c>
@@ -5643,18 +5654,18 @@
       <c r="U10" s="30"/>
     </row>
     <row r="11" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J11" s="206" t="s">
+      <c r="J11" s="212" t="s">
         <v>80</v>
       </c>
-      <c r="K11" s="207"/>
-      <c r="L11" s="207"/>
-      <c r="M11" s="207"/>
-      <c r="N11" s="208"/>
-      <c r="Q11" s="210"/>
+      <c r="K11" s="213"/>
+      <c r="L11" s="213"/>
+      <c r="M11" s="213"/>
+      <c r="N11" s="214"/>
+      <c r="Q11" s="216"/>
       <c r="R11" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="S11" s="188"/>
+      <c r="S11" s="187"/>
       <c r="T11" s="23"/>
       <c r="U11" s="25"/>
     </row>
@@ -5674,14 +5685,14 @@
       <c r="N12" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="Q12" s="210"/>
+      <c r="Q12" s="216"/>
       <c r="R12" s="23" t="s">
         <v>7</v>
       </c>
       <c r="S12" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="T12" s="189">
+      <c r="T12" s="188">
         <v>409.71</v>
       </c>
       <c r="U12" s="25" t="s">
@@ -5707,7 +5718,7 @@
         <f>M13/25.4</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="210"/>
+      <c r="Q13" s="216"/>
       <c r="R13" s="23" t="s">
         <v>10</v>
       </c>
@@ -5736,7 +5747,7 @@
         <f t="shared" ref="N14:N32" si="2">M14/25.4</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="210"/>
+      <c r="Q14" s="216"/>
       <c r="R14" s="3" t="s">
         <v>11</v>
       </c>
@@ -5759,7 +5770,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M15" s="247">
+      <c r="M15" s="204">
         <f>315.69/2</f>
         <v>157.845</v>
       </c>
@@ -5768,7 +5779,7 @@
         <v>6.2143700787401581</v>
       </c>
       <c r="O15" s="178"/>
-      <c r="Q15" s="210"/>
+      <c r="Q15" s="216"/>
       <c r="R15" s="6" t="s">
         <v>16</v>
       </c>
@@ -5787,7 +5798,7 @@
         <f t="shared" si="1"/>
         <v>48.031496062992126</v>
       </c>
-      <c r="M16" s="247">
+      <c r="M16" s="204">
         <f>315.69/2</f>
         <v>157.845</v>
       </c>
@@ -5795,11 +5806,11 @@
         <f t="shared" si="2"/>
         <v>6.2143700787401581</v>
       </c>
-      <c r="Q16" s="210"/>
+      <c r="Q16" s="216"/>
       <c r="R16" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="S16" s="188"/>
+      <c r="S16" s="187"/>
       <c r="T16" s="23"/>
       <c r="U16" s="25"/>
     </row>
@@ -5814,7 +5825,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M17" s="247">
+      <c r="M17" s="204">
         <f>631.37/2</f>
         <v>315.685</v>
       </c>
@@ -5823,14 +5834,14 @@
         <v>12.428543307086615</v>
       </c>
       <c r="O17" s="178"/>
-      <c r="Q17" s="210"/>
+      <c r="Q17" s="216"/>
       <c r="R17" s="23" t="s">
         <v>7</v>
       </c>
       <c r="S17" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="T17" s="189">
+      <c r="T17" s="188">
         <v>429.78</v>
       </c>
       <c r="U17" s="25" t="s">
@@ -5848,7 +5859,7 @@
         <f t="shared" si="1"/>
         <v>48.031496062992126</v>
       </c>
-      <c r="M18" s="247">
+      <c r="M18" s="204">
         <f>631.37/2</f>
         <v>315.685</v>
       </c>
@@ -5856,7 +5867,7 @@
         <f t="shared" si="2"/>
         <v>12.428543307086615</v>
       </c>
-      <c r="Q18" s="210"/>
+      <c r="Q18" s="216"/>
       <c r="R18" s="23" t="s">
         <v>10</v>
       </c>
@@ -5886,7 +5897,7 @@
         <v>18.642913385826773</v>
       </c>
       <c r="O19" s="178"/>
-      <c r="Q19" s="210"/>
+      <c r="Q19" s="216"/>
       <c r="R19" s="3" t="s">
         <v>11</v>
       </c>
@@ -5918,7 +5929,7 @@
         <f t="shared" si="2"/>
         <v>18.642913385826773</v>
       </c>
-      <c r="Q20" s="210"/>
+      <c r="Q20" s="216"/>
       <c r="R20" s="32" t="s">
         <v>19</v>
       </c>
@@ -5952,7 +5963,7 @@
         <v>24.85708661417323</v>
       </c>
       <c r="O21" s="178"/>
-      <c r="Q21" s="210"/>
+      <c r="Q21" s="216"/>
       <c r="R21" s="32" t="s">
         <v>21</v>
       </c>
@@ -5983,7 +5994,7 @@
         <f t="shared" si="2"/>
         <v>24.85708661417323</v>
       </c>
-      <c r="Q22" s="210"/>
+      <c r="Q22" s="216"/>
       <c r="R22" s="32" t="s">
         <v>24</v>
       </c>
@@ -6006,7 +6017,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M23" s="247">
+      <c r="M23" s="204">
         <f>1578.43/2</f>
         <v>789.21500000000003</v>
       </c>
@@ -6015,7 +6026,7 @@
         <v>31.07145669291339</v>
       </c>
       <c r="O23" s="178"/>
-      <c r="Q23" s="211"/>
+      <c r="Q23" s="217"/>
       <c r="R23" s="2"/>
       <c r="S23" s="8" t="s">
         <v>26</v>
@@ -6036,7 +6047,7 @@
         <f t="shared" si="1"/>
         <v>48.031496062992126</v>
       </c>
-      <c r="M24" s="247">
+      <c r="M24" s="204">
         <f>1578.43/2</f>
         <v>789.21500000000003</v>
       </c>
@@ -6044,7 +6055,7 @@
         <f t="shared" si="2"/>
         <v>31.07145669291339</v>
       </c>
-      <c r="Q24" s="212" t="s">
+      <c r="Q24" s="218" t="s">
         <v>27</v>
       </c>
       <c r="R24" s="1" t="s">
@@ -6067,7 +6078,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M25" s="247">
+      <c r="M25" s="204">
         <f>1894.11/2</f>
         <v>947.05499999999995</v>
       </c>
@@ -6076,7 +6087,7 @@
         <v>37.28562992125984</v>
       </c>
       <c r="O25" s="178"/>
-      <c r="Q25" s="210"/>
+      <c r="Q25" s="216"/>
       <c r="R25" s="6" t="s">
         <v>29</v>
       </c>
@@ -6095,7 +6106,7 @@
         <f t="shared" si="1"/>
         <v>48.031496062992126</v>
       </c>
-      <c r="M26" s="247">
+      <c r="M26" s="204">
         <f>1894.11/2</f>
         <v>947.05499999999995</v>
       </c>
@@ -6103,7 +6114,7 @@
         <f t="shared" si="2"/>
         <v>37.28562992125984</v>
       </c>
-      <c r="Q26" s="210"/>
+      <c r="Q26" s="216"/>
       <c r="R26" s="23" t="s">
         <v>30</v>
       </c>
@@ -6137,7 +6148,7 @@
         <v>43.500000000000007</v>
       </c>
       <c r="O27" s="178"/>
-      <c r="Q27" s="210"/>
+      <c r="Q27" s="216"/>
       <c r="R27" s="23" t="s">
         <v>32</v>
       </c>
@@ -6168,14 +6179,14 @@
         <f t="shared" si="2"/>
         <v>43.500000000000007</v>
       </c>
-      <c r="Q28" s="210"/>
+      <c r="Q28" s="216"/>
       <c r="R28" s="23" t="s">
         <v>19</v>
       </c>
       <c r="S28" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="T28" s="194">
+      <c r="T28" s="193">
         <f>4700*SQRT(-T26)</f>
         <v>32252.412312879791</v>
       </c>
@@ -6194,7 +6205,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M29" s="199">
+      <c r="M29" s="198">
         <f>2438.4/2</f>
         <v>1219.2</v>
       </c>
@@ -6203,14 +6214,14 @@
         <v>48.000000000000007</v>
       </c>
       <c r="O29" s="178"/>
-      <c r="Q29" s="210"/>
+      <c r="Q29" s="216"/>
       <c r="R29" s="23" t="s">
         <v>34</v>
       </c>
       <c r="S29" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="T29" s="193">
+      <c r="T29" s="192">
         <v>1.02</v>
       </c>
       <c r="U29" s="88"/>
@@ -6227,7 +6238,7 @@
         <f t="shared" si="1"/>
         <v>48.031496062992126</v>
       </c>
-      <c r="M30" s="199">
+      <c r="M30" s="198">
         <f>2438.4/2</f>
         <v>1219.2</v>
       </c>
@@ -6235,18 +6246,18 @@
         <f t="shared" si="2"/>
         <v>48.000000000000007</v>
       </c>
-      <c r="Q30" s="210"/>
+      <c r="Q30" s="216"/>
       <c r="R30" s="23" t="s">
         <v>36</v>
       </c>
       <c r="S30" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="T30" s="192">
+      <c r="T30" s="191">
         <f>(-T26/5.2-1.9)</f>
         <v>7.1557692307692307</v>
       </c>
-      <c r="U30" s="191"/>
+      <c r="U30" s="190"/>
     </row>
     <row r="31" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J31" s="14">
@@ -6268,7 +6279,7 @@
         <v>52.5</v>
       </c>
       <c r="O31" s="178"/>
-      <c r="Q31" s="210"/>
+      <c r="Q31" s="216"/>
       <c r="R31" s="6" t="s">
         <v>37</v>
       </c>
@@ -6287,7 +6298,7 @@
         <f t="shared" si="1"/>
         <v>48.031496062992126</v>
       </c>
-      <c r="M32" s="248">
+      <c r="M32" s="205">
         <f>2667/2</f>
         <v>1333.5</v>
       </c>
@@ -6295,7 +6306,7 @@
         <f t="shared" si="2"/>
         <v>52.5</v>
       </c>
-      <c r="Q32" s="210"/>
+      <c r="Q32" s="216"/>
       <c r="R32" s="23" t="s">
         <v>38</v>
       </c>
@@ -6310,7 +6321,7 @@
       </c>
     </row>
     <row r="33" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q33" s="210"/>
+      <c r="Q33" s="216"/>
       <c r="R33" s="23" t="s">
         <v>40</v>
       </c>
@@ -6323,14 +6334,14 @@
       <c r="U33" s="25"/>
     </row>
     <row r="34" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q34" s="210"/>
+      <c r="Q34" s="216"/>
       <c r="R34" s="23" t="s">
         <v>42</v>
       </c>
       <c r="S34" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="T34" s="194">
+      <c r="T34" s="193">
         <f>4700*SQRT(-T32)</f>
         <v>34467.378780522318</v>
       </c>
@@ -6339,34 +6350,34 @@
       </c>
     </row>
     <row r="35" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q35" s="210"/>
+      <c r="Q35" s="216"/>
       <c r="R35" s="23" t="s">
         <v>34</v>
       </c>
       <c r="S35" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="T35" s="193">
+      <c r="T35" s="192">
         <v>1.02</v>
       </c>
       <c r="U35" s="25"/>
     </row>
     <row r="36" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q36" s="210"/>
+      <c r="Q36" s="216"/>
       <c r="R36" s="23" t="s">
         <v>36</v>
       </c>
       <c r="S36" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="T36" s="192">
+      <c r="T36" s="191">
         <f>(-T32/5.2-1.9)</f>
         <v>8.4423076923076916</v>
       </c>
-      <c r="U36" s="191"/>
+      <c r="U36" s="190"/>
     </row>
     <row r="37" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q37" s="210"/>
+      <c r="Q37" s="216"/>
       <c r="R37" s="6" t="s">
         <v>44</v>
       </c>
@@ -6375,14 +6386,14 @@
       <c r="U37" s="30"/>
     </row>
     <row r="38" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q38" s="210"/>
+      <c r="Q38" s="216"/>
       <c r="R38" s="23" t="s">
         <v>45</v>
       </c>
       <c r="S38" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="T38" s="190">
+      <c r="T38" s="189">
         <f>0.31*SQRT(-T26)</f>
         <v>2.1272867695729225</v>
       </c>
@@ -6391,7 +6402,7 @@
       </c>
     </row>
     <row r="39" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q39" s="210"/>
+      <c r="Q39" s="216"/>
       <c r="R39" s="23" t="s">
         <v>46</v>
       </c>
@@ -6404,7 +6415,7 @@
       <c r="U39" s="25"/>
     </row>
     <row r="40" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q40" s="210"/>
+      <c r="Q40" s="216"/>
       <c r="R40" s="23" t="s">
         <v>34</v>
       </c>
@@ -6419,7 +6430,7 @@
       </c>
     </row>
     <row r="41" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q41" s="211"/>
+      <c r="Q41" s="217"/>
       <c r="R41" s="23" t="s">
         <v>36</v>
       </c>
@@ -6432,7 +6443,7 @@
       <c r="U41" s="22"/>
     </row>
     <row r="42" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q42" s="213" t="s">
+      <c r="Q42" s="219" t="s">
         <v>50</v>
       </c>
       <c r="R42" s="6" t="s">
@@ -6445,7 +6456,7 @@
       <c r="U42" s="30"/>
     </row>
     <row r="43" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q43" s="201"/>
+      <c r="Q43" s="207"/>
       <c r="R43" s="6" t="s">
         <v>52</v>
       </c>
@@ -6454,7 +6465,7 @@
       <c r="U43" s="30"/>
     </row>
     <row r="44" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q44" s="201"/>
+      <c r="Q44" s="207"/>
       <c r="R44" s="23" t="s">
         <v>53</v>
       </c>
@@ -6465,7 +6476,7 @@
       <c r="U44" s="25"/>
     </row>
     <row r="45" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q45" s="201"/>
+      <c r="Q45" s="207"/>
       <c r="R45" s="23" t="s">
         <v>54</v>
       </c>
@@ -6480,7 +6491,7 @@
       </c>
     </row>
     <row r="46" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q46" s="201"/>
+      <c r="Q46" s="207"/>
       <c r="R46" s="23" t="s">
         <v>57</v>
       </c>
@@ -6495,7 +6506,7 @@
       </c>
     </row>
     <row r="47" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q47" s="201"/>
+      <c r="Q47" s="207"/>
       <c r="R47" s="23" t="s">
         <v>59</v>
       </c>
@@ -6511,7 +6522,7 @@
       </c>
     </row>
     <row r="48" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q48" s="201"/>
+      <c r="Q48" s="207"/>
       <c r="R48" s="23"/>
       <c r="S48" s="26" t="s">
         <v>306</v>
@@ -6523,7 +6534,7 @@
       <c r="U48" s="25"/>
     </row>
     <row r="49" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q49" s="201"/>
+      <c r="Q49" s="207"/>
       <c r="R49" s="23" t="s">
         <v>61</v>
       </c>
@@ -6537,7 +6548,7 @@
       <c r="U49" s="25"/>
     </row>
     <row r="50" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q50" s="201"/>
+      <c r="Q50" s="207"/>
       <c r="R50" s="6" t="s">
         <v>62</v>
       </c>
@@ -6549,7 +6560,7 @@
       <c r="H51" s="15"/>
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
-      <c r="Q51" s="201"/>
+      <c r="Q51" s="207"/>
       <c r="R51" s="23" t="s">
         <v>63</v>
       </c>
@@ -6564,7 +6575,7 @@
       <c r="I52" s="15"/>
       <c r="J52" s="15"/>
       <c r="N52" s="144"/>
-      <c r="Q52" s="201"/>
+      <c r="Q52" s="207"/>
       <c r="R52" s="23" t="s">
         <v>54</v>
       </c>
@@ -6582,7 +6593,7 @@
       <c r="H53" s="15"/>
       <c r="I53" s="15"/>
       <c r="J53" s="15"/>
-      <c r="Q53" s="201"/>
+      <c r="Q53" s="207"/>
       <c r="R53" s="23" t="s">
         <v>64</v>
       </c>
@@ -6598,7 +6609,7 @@
       </c>
     </row>
     <row r="54" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q54" s="201"/>
+      <c r="Q54" s="207"/>
       <c r="R54" s="23" t="s">
         <v>66</v>
       </c>
@@ -6614,7 +6625,7 @@
       </c>
     </row>
     <row r="55" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q55" s="201"/>
+      <c r="Q55" s="207"/>
       <c r="R55" s="23" t="s">
         <v>61</v>
       </c>
@@ -6628,7 +6639,7 @@
       <c r="U55" s="25"/>
     </row>
     <row r="56" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q56" s="201"/>
+      <c r="Q56" s="207"/>
       <c r="R56" s="6" t="s">
         <v>69</v>
       </c>
@@ -6637,7 +6648,7 @@
       <c r="U56" s="30"/>
     </row>
     <row r="57" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q57" s="201"/>
+      <c r="Q57" s="207"/>
       <c r="R57" s="23" t="s">
         <v>70</v>
       </c>
@@ -6648,7 +6659,7 @@
       <c r="U57" s="25"/>
     </row>
     <row r="58" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q58" s="201"/>
+      <c r="Q58" s="207"/>
       <c r="R58" s="23" t="s">
         <v>54</v>
       </c>
@@ -6664,7 +6675,7 @@
       <c r="V58" s="27"/>
     </row>
     <row r="59" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q59" s="201"/>
+      <c r="Q59" s="207"/>
       <c r="R59" s="23" t="s">
         <v>57</v>
       </c>
@@ -6679,7 +6690,7 @@
       </c>
     </row>
     <row r="60" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q60" s="201"/>
+      <c r="Q60" s="207"/>
       <c r="R60" s="23" t="s">
         <v>71</v>
       </c>
@@ -6692,7 +6703,7 @@
       <c r="U60" s="25"/>
     </row>
     <row r="61" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q61" s="201"/>
+      <c r="Q61" s="207"/>
       <c r="R61" s="23" t="s">
         <v>59</v>
       </c>
@@ -6709,7 +6720,7 @@
       <c r="V61" s="37"/>
     </row>
     <row r="62" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q62" s="201"/>
+      <c r="Q62" s="207"/>
       <c r="R62" s="23" t="s">
         <v>61</v>
       </c>
@@ -6721,10 +6732,10 @@
         <v>8.3105763874489758E-3</v>
       </c>
       <c r="U62" s="25"/>
-      <c r="V62" s="195"/>
+      <c r="V62" s="194"/>
     </row>
     <row r="63" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q63" s="201"/>
+      <c r="Q63" s="207"/>
       <c r="R63" s="6" t="s">
         <v>73</v>
       </c>
@@ -6733,7 +6744,7 @@
       <c r="U63" s="30"/>
     </row>
     <row r="64" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q64" s="201"/>
+      <c r="Q64" s="207"/>
       <c r="R64" s="23" t="s">
         <v>74</v>
       </c>
@@ -6748,7 +6759,7 @@
       </c>
     </row>
     <row r="65" spans="17:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q65" s="202"/>
+      <c r="Q65" s="208"/>
       <c r="R65" s="40" t="s">
         <v>77</v>
       </c>
@@ -6763,7 +6774,7 @@
       </c>
     </row>
     <row r="66" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q66" s="200" t="s">
+      <c r="Q66" s="206" t="s">
         <v>346</v>
       </c>
       <c r="R66" s="18" t="s">
@@ -6776,7 +6787,7 @@
       <c r="U66" s="21"/>
     </row>
     <row r="67" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q67" s="201"/>
+      <c r="Q67" s="207"/>
       <c r="R67" s="6" t="s">
         <v>83</v>
       </c>
@@ -6785,7 +6796,7 @@
       <c r="U67" s="30"/>
     </row>
     <row r="68" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q68" s="201"/>
+      <c r="Q68" s="207"/>
       <c r="R68" s="23" t="s">
         <v>81</v>
       </c>
@@ -6798,7 +6809,7 @@
       <c r="U68" s="45"/>
     </row>
     <row r="69" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q69" s="201"/>
+      <c r="Q69" s="207"/>
       <c r="R69" s="2" t="s">
         <v>86</v>
       </c>
@@ -6811,7 +6822,7 @@
       </c>
     </row>
     <row r="70" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q70" s="201"/>
+      <c r="Q70" s="207"/>
       <c r="R70" s="6" t="s">
         <v>84</v>
       </c>
@@ -6820,7 +6831,7 @@
       <c r="U70" s="49"/>
     </row>
     <row r="71" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q71" s="201"/>
+      <c r="Q71" s="207"/>
       <c r="R71" s="23" t="s">
         <v>85</v>
       </c>
@@ -6833,7 +6844,7 @@
       <c r="U71" s="45"/>
     </row>
     <row r="72" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q72" s="201"/>
+      <c r="Q72" s="207"/>
       <c r="R72" s="23" t="s">
         <v>89</v>
       </c>
@@ -6848,7 +6859,7 @@
       </c>
     </row>
     <row r="73" spans="17:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q73" s="202"/>
+      <c r="Q73" s="208"/>
       <c r="R73" s="40"/>
       <c r="S73" s="41" t="s">
         <v>88</v>
@@ -6898,10 +6909,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C3" s="217" t="s">
+      <c r="C3" s="223" t="s">
         <v>215</v>
       </c>
-      <c r="D3" s="217" t="s">
+      <c r="D3" s="223" t="s">
         <v>91</v>
       </c>
       <c r="E3" s="82">
@@ -6913,8 +6924,8 @@
       </c>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C4" s="217"/>
-      <c r="D4" s="217"/>
+      <c r="C4" s="223"/>
+      <c r="D4" s="223"/>
       <c r="E4" s="84">
         <f>E3*9.807</f>
         <v>-2145185.2167177605</v>
@@ -6928,7 +6939,7 @@
       </c>
     </row>
     <row r="8" spans="3:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="218">
+      <c r="C8" s="224">
         <v>1</v>
       </c>
       <c r="D8" s="147" t="s">
@@ -6941,7 +6952,7 @@
       <c r="G8" s="150"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C9" s="219"/>
+      <c r="C9" s="225"/>
       <c r="D9" s="151" t="s">
         <v>111</v>
       </c>
@@ -6950,7 +6961,7 @@
       <c r="G9" s="153"/>
     </row>
     <row r="10" spans="3:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="C10" s="219"/>
+      <c r="C10" s="225"/>
       <c r="D10" s="154" t="s">
         <v>34</v>
       </c>
@@ -6963,7 +6974,7 @@
       <c r="G10" s="157"/>
     </row>
     <row r="11" spans="3:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="C11" s="219"/>
+      <c r="C11" s="225"/>
       <c r="D11" s="151" t="s">
         <v>113</v>
       </c>
@@ -6972,7 +6983,7 @@
       <c r="G11" s="157"/>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C12" s="219"/>
+      <c r="C12" s="225"/>
       <c r="D12" s="154" t="s">
         <v>114</v>
       </c>
@@ -6985,7 +6996,7 @@
       <c r="G12" s="153"/>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C13" s="219"/>
+      <c r="C13" s="225"/>
       <c r="D13" s="151" t="s">
         <v>112</v>
       </c>
@@ -6997,7 +7008,7 @@
       </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C14" s="219"/>
+      <c r="C14" s="225"/>
       <c r="D14" s="154" t="s">
         <v>98</v>
       </c>
@@ -7014,7 +7025,7 @@
       </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C15" s="219"/>
+      <c r="C15" s="225"/>
       <c r="D15" s="154" t="s">
         <v>97</v>
       </c>
@@ -7030,11 +7041,11 @@
       </c>
       <c r="J15" s="50">
         <f>'Prop Geom y de Materiales'!M9*'Parámetros de Análisis'!I15/100</f>
-        <v>0</v>
+        <v>5.4344262295081963E-2</v>
       </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C16" s="219"/>
+      <c r="C16" s="225"/>
       <c r="D16" s="154" t="s">
         <v>102</v>
       </c>
@@ -7047,7 +7058,7 @@
       <c r="G16" s="153"/>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C17" s="219"/>
+      <c r="C17" s="225"/>
       <c r="D17" s="154" t="s">
         <v>103</v>
       </c>
@@ -7060,7 +7071,7 @@
       <c r="G17" s="153"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C18" s="219"/>
+      <c r="C18" s="225"/>
       <c r="D18" s="154" t="s">
         <v>94</v>
       </c>
@@ -7073,7 +7084,7 @@
       <c r="G18" s="153"/>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C19" s="219"/>
+      <c r="C19" s="225"/>
       <c r="D19" s="161" t="s">
         <v>95</v>
       </c>
@@ -7086,7 +7097,7 @@
       <c r="G19" s="164"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C20" s="219"/>
+      <c r="C20" s="225"/>
       <c r="D20" s="147" t="s">
         <v>116</v>
       </c>
@@ -7097,7 +7108,7 @@
       <c r="G20" s="150"/>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C21" s="219"/>
+      <c r="C21" s="225"/>
       <c r="D21" s="154" t="s">
         <v>119</v>
       </c>
@@ -7108,7 +7119,7 @@
       <c r="G21" s="153"/>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C22" s="219"/>
+      <c r="C22" s="225"/>
       <c r="D22" s="161" t="s">
         <v>121</v>
       </c>
@@ -7119,7 +7130,7 @@
       <c r="G22" s="164"/>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C23" s="219"/>
+      <c r="C23" s="225"/>
       <c r="D23" s="147" t="s">
         <v>116</v>
       </c>
@@ -7130,7 +7141,7 @@
       <c r="G23" s="150"/>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C24" s="219"/>
+      <c r="C24" s="225"/>
       <c r="D24" s="154" t="s">
         <v>126</v>
       </c>
@@ -7143,7 +7154,7 @@
       <c r="G24" s="153"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C25" s="219"/>
+      <c r="C25" s="225"/>
       <c r="D25" s="154" t="s">
         <v>119</v>
       </c>
@@ -7156,7 +7167,7 @@
       <c r="G25" s="153"/>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C26" s="220"/>
+      <c r="C26" s="226"/>
       <c r="D26" s="161" t="s">
         <v>110</v>
       </c>
@@ -7169,7 +7180,7 @@
       <c r="G26" s="164"/>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C27" s="214" t="s">
+      <c r="C27" s="220" t="s">
         <v>307</v>
       </c>
       <c r="D27" s="65" t="s">
@@ -7182,14 +7193,14 @@
       <c r="G27" s="68"/>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C28" s="215"/>
+      <c r="C28" s="221"/>
       <c r="D28" s="54" t="s">
         <v>111</v>
       </c>
       <c r="G28" s="55"/>
     </row>
     <row r="29" spans="3:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="C29" s="215"/>
+      <c r="C29" s="221"/>
       <c r="D29" s="56" t="s">
         <v>34</v>
       </c>
@@ -7202,7 +7213,7 @@
       <c r="G29" s="57"/>
     </row>
     <row r="30" spans="3:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="C30" s="215"/>
+      <c r="C30" s="221"/>
       <c r="D30" s="54" t="s">
         <v>113</v>
       </c>
@@ -7211,7 +7222,7 @@
       <c r="G30" s="57"/>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C31" s="215"/>
+      <c r="C31" s="221"/>
       <c r="D31" s="56" t="s">
         <v>114</v>
       </c>
@@ -7226,14 +7237,14 @@
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C32" s="215"/>
+      <c r="C32" s="221"/>
       <c r="D32" s="54" t="s">
         <v>112</v>
       </c>
       <c r="G32" s="55"/>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C33" s="215"/>
+      <c r="C33" s="221"/>
       <c r="D33" s="56" t="s">
         <v>98</v>
       </c>
@@ -7244,7 +7255,7 @@
       <c r="G33" s="55"/>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C34" s="215"/>
+      <c r="C34" s="221"/>
       <c r="D34" s="56" t="s">
         <v>97</v>
       </c>
@@ -7257,7 +7268,7 @@
       <c r="G34" s="55"/>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C35" s="215"/>
+      <c r="C35" s="221"/>
       <c r="D35" s="56" t="s">
         <v>102</v>
       </c>
@@ -7270,7 +7281,7 @@
       <c r="G35" s="55"/>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C36" s="215"/>
+      <c r="C36" s="221"/>
       <c r="D36" s="56" t="s">
         <v>103</v>
       </c>
@@ -7283,7 +7294,7 @@
       <c r="G36" s="55"/>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C37" s="215"/>
+      <c r="C37" s="221"/>
       <c r="D37" s="56" t="s">
         <v>94</v>
       </c>
@@ -7296,7 +7307,7 @@
       <c r="G37" s="55"/>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C38" s="215"/>
+      <c r="C38" s="221"/>
       <c r="D38" s="60" t="s">
         <v>95</v>
       </c>
@@ -7309,7 +7320,7 @@
       <c r="G38" s="63"/>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C39" s="215"/>
+      <c r="C39" s="221"/>
       <c r="D39" s="65" t="s">
         <v>116</v>
       </c>
@@ -7320,7 +7331,7 @@
       <c r="G39" s="68"/>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C40" s="215"/>
+      <c r="C40" s="221"/>
       <c r="D40" s="56" t="s">
         <v>119</v>
       </c>
@@ -7330,7 +7341,7 @@
       <c r="G40" s="55"/>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C41" s="215"/>
+      <c r="C41" s="221"/>
       <c r="D41" s="60" t="s">
         <v>121</v>
       </c>
@@ -7341,7 +7352,7 @@
       <c r="G41" s="63"/>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C42" s="215"/>
+      <c r="C42" s="221"/>
       <c r="D42" s="65" t="s">
         <v>116</v>
       </c>
@@ -7352,7 +7363,7 @@
       <c r="G42" s="68"/>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C43" s="215"/>
+      <c r="C43" s="221"/>
       <c r="D43" s="56" t="s">
         <v>126</v>
       </c>
@@ -7365,7 +7376,7 @@
       <c r="G43" s="55"/>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C44" s="215"/>
+      <c r="C44" s="221"/>
       <c r="D44" s="56" t="s">
         <v>119</v>
       </c>
@@ -7378,7 +7389,7 @@
       <c r="G44" s="55"/>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C45" s="216"/>
+      <c r="C45" s="222"/>
       <c r="D45" s="60" t="s">
         <v>110</v>
       </c>
@@ -7391,7 +7402,7 @@
       <c r="G45" s="63"/>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C46" s="214" t="s">
+      <c r="C46" s="220" t="s">
         <v>308</v>
       </c>
       <c r="D46" s="65" t="s">
@@ -7404,14 +7415,14 @@
       <c r="G46" s="68"/>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C47" s="215"/>
+      <c r="C47" s="221"/>
       <c r="D47" s="54" t="s">
         <v>111</v>
       </c>
       <c r="G47" s="55"/>
     </row>
     <row r="48" spans="3:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="C48" s="215"/>
+      <c r="C48" s="221"/>
       <c r="D48" s="56" t="s">
         <v>34</v>
       </c>
@@ -7424,7 +7435,7 @@
       <c r="G48" s="57"/>
     </row>
     <row r="49" spans="3:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="C49" s="215"/>
+      <c r="C49" s="221"/>
       <c r="D49" s="54" t="s">
         <v>113</v>
       </c>
@@ -7433,7 +7444,7 @@
       <c r="G49" s="57"/>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C50" s="215"/>
+      <c r="C50" s="221"/>
       <c r="D50" s="56" t="s">
         <v>114</v>
       </c>
@@ -7448,14 +7459,14 @@
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C51" s="215"/>
+      <c r="C51" s="221"/>
       <c r="D51" s="54" t="s">
         <v>112</v>
       </c>
       <c r="G51" s="55"/>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C52" s="215"/>
+      <c r="C52" s="221"/>
       <c r="D52" s="56" t="s">
         <v>98</v>
       </c>
@@ -7466,7 +7477,7 @@
       <c r="G52" s="55"/>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C53" s="215"/>
+      <c r="C53" s="221"/>
       <c r="D53" s="56" t="s">
         <v>97</v>
       </c>
@@ -7479,7 +7490,7 @@
       <c r="G53" s="55"/>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C54" s="215"/>
+      <c r="C54" s="221"/>
       <c r="D54" s="56" t="s">
         <v>102</v>
       </c>
@@ -7492,7 +7503,7 @@
       <c r="G54" s="55"/>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C55" s="215"/>
+      <c r="C55" s="221"/>
       <c r="D55" s="56" t="s">
         <v>103</v>
       </c>
@@ -7505,7 +7516,7 @@
       <c r="G55" s="55"/>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C56" s="215"/>
+      <c r="C56" s="221"/>
       <c r="D56" s="56" t="s">
         <v>94</v>
       </c>
@@ -7518,7 +7529,7 @@
       <c r="G56" s="55"/>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C57" s="215"/>
+      <c r="C57" s="221"/>
       <c r="D57" s="60" t="s">
         <v>95</v>
       </c>
@@ -7531,7 +7542,7 @@
       <c r="G57" s="63"/>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C58" s="215"/>
+      <c r="C58" s="221"/>
       <c r="D58" s="65" t="s">
         <v>116</v>
       </c>
@@ -7542,7 +7553,7 @@
       <c r="G58" s="68"/>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C59" s="215"/>
+      <c r="C59" s="221"/>
       <c r="D59" s="56" t="s">
         <v>119</v>
       </c>
@@ -7552,7 +7563,7 @@
       <c r="G59" s="55"/>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C60" s="215"/>
+      <c r="C60" s="221"/>
       <c r="D60" s="60" t="s">
         <v>121</v>
       </c>
@@ -7563,7 +7574,7 @@
       <c r="G60" s="63"/>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C61" s="215"/>
+      <c r="C61" s="221"/>
       <c r="D61" s="65" t="s">
         <v>116</v>
       </c>
@@ -7574,7 +7585,7 @@
       <c r="G61" s="68"/>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C62" s="215"/>
+      <c r="C62" s="221"/>
       <c r="D62" s="56" t="s">
         <v>126</v>
       </c>
@@ -7587,7 +7598,7 @@
       <c r="G62" s="55"/>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C63" s="215"/>
+      <c r="C63" s="221"/>
       <c r="D63" s="56" t="s">
         <v>119</v>
       </c>
@@ -7600,7 +7611,7 @@
       <c r="G63" s="55"/>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C64" s="216"/>
+      <c r="C64" s="222"/>
       <c r="D64" s="60" t="s">
         <v>110</v>
       </c>
@@ -7613,7 +7624,7 @@
       <c r="G64" s="63"/>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C65" s="214" t="s">
+      <c r="C65" s="220" t="s">
         <v>309</v>
       </c>
       <c r="D65" s="65" t="s">
@@ -7626,14 +7637,14 @@
       <c r="G65" s="68"/>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C66" s="215"/>
+      <c r="C66" s="221"/>
       <c r="D66" s="54" t="s">
         <v>111</v>
       </c>
       <c r="G66" s="55"/>
     </row>
     <row r="67" spans="3:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="C67" s="215"/>
+      <c r="C67" s="221"/>
       <c r="D67" s="56" t="s">
         <v>34</v>
       </c>
@@ -7646,7 +7657,7 @@
       <c r="G67" s="57"/>
     </row>
     <row r="68" spans="3:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="C68" s="215"/>
+      <c r="C68" s="221"/>
       <c r="D68" s="54" t="s">
         <v>113</v>
       </c>
@@ -7655,7 +7666,7 @@
       <c r="G68" s="57"/>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C69" s="215"/>
+      <c r="C69" s="221"/>
       <c r="D69" s="56" t="s">
         <v>114</v>
       </c>
@@ -7671,14 +7682,14 @@
       </c>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C70" s="215"/>
+      <c r="C70" s="221"/>
       <c r="D70" s="54" t="s">
         <v>112</v>
       </c>
       <c r="G70" s="55"/>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C71" s="215"/>
+      <c r="C71" s="221"/>
       <c r="D71" s="56" t="s">
         <v>98</v>
       </c>
@@ -7689,7 +7700,7 @@
       <c r="G71" s="55"/>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C72" s="215"/>
+      <c r="C72" s="221"/>
       <c r="D72" s="56" t="s">
         <v>97</v>
       </c>
@@ -7702,7 +7713,7 @@
       <c r="G72" s="55"/>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C73" s="215"/>
+      <c r="C73" s="221"/>
       <c r="D73" s="56" t="s">
         <v>102</v>
       </c>
@@ -7715,7 +7726,7 @@
       <c r="G73" s="55"/>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C74" s="215"/>
+      <c r="C74" s="221"/>
       <c r="D74" s="56" t="s">
         <v>103</v>
       </c>
@@ -7728,7 +7739,7 @@
       <c r="G74" s="55"/>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C75" s="215"/>
+      <c r="C75" s="221"/>
       <c r="D75" s="56" t="s">
         <v>94</v>
       </c>
@@ -7741,7 +7752,7 @@
       <c r="G75" s="55"/>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C76" s="215"/>
+      <c r="C76" s="221"/>
       <c r="D76" s="60" t="s">
         <v>95</v>
       </c>
@@ -7754,7 +7765,7 @@
       <c r="G76" s="63"/>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C77" s="215"/>
+      <c r="C77" s="221"/>
       <c r="D77" s="65" t="s">
         <v>116</v>
       </c>
@@ -7765,7 +7776,7 @@
       <c r="G77" s="68"/>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C78" s="215"/>
+      <c r="C78" s="221"/>
       <c r="D78" s="56" t="s">
         <v>119</v>
       </c>
@@ -7775,7 +7786,7 @@
       <c r="G78" s="55"/>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C79" s="215"/>
+      <c r="C79" s="221"/>
       <c r="D79" s="60" t="s">
         <v>121</v>
       </c>
@@ -7786,7 +7797,7 @@
       <c r="G79" s="63"/>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C80" s="215"/>
+      <c r="C80" s="221"/>
       <c r="D80" s="65" t="s">
         <v>116</v>
       </c>
@@ -7797,7 +7808,7 @@
       <c r="G80" s="68"/>
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C81" s="215"/>
+      <c r="C81" s="221"/>
       <c r="D81" s="56" t="s">
         <v>126</v>
       </c>
@@ -7810,7 +7821,7 @@
       <c r="G81" s="55"/>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C82" s="215"/>
+      <c r="C82" s="221"/>
       <c r="D82" s="56" t="s">
         <v>119</v>
       </c>
@@ -7823,7 +7834,7 @@
       <c r="G82" s="55"/>
     </row>
     <row r="83" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C83" s="216"/>
+      <c r="C83" s="222"/>
       <c r="D83" s="60" t="s">
         <v>110</v>
       </c>
@@ -7854,8 +7865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AK323"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="O146" sqref="O146"/>
+    <sheetView topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G131" sqref="G131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7917,12 +7928,12 @@
       <c r="V8" s="75"/>
     </row>
     <row r="9" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D9" s="225" t="s">
+      <c r="D9" s="231" t="s">
         <v>177</v>
       </c>
-      <c r="E9" s="226"/>
-      <c r="F9" s="226"/>
-      <c r="G9" s="227"/>
+      <c r="E9" s="232"/>
+      <c r="F9" s="232"/>
+      <c r="G9" s="233"/>
       <c r="V9" s="75"/>
     </row>
     <row r="10" spans="4:23" x14ac:dyDescent="0.25">
@@ -8096,7 +8107,7 @@
       </c>
     </row>
     <row r="17" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D17" s="201" t="s">
+      <c r="D17" s="207" t="s">
         <v>59</v>
       </c>
       <c r="E17" s="69" t="s">
@@ -8120,7 +8131,7 @@
       <c r="V17" s="75"/>
     </row>
     <row r="18" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D18" s="201"/>
+      <c r="D18" s="207"/>
       <c r="E18" s="69" t="s">
         <v>140</v>
       </c>
@@ -8142,7 +8153,7 @@
       <c r="V18" s="75"/>
     </row>
     <row r="19" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D19" s="201"/>
+      <c r="D19" s="207"/>
       <c r="E19" s="69" t="s">
         <v>141</v>
       </c>
@@ -8268,7 +8279,7 @@
       <c r="D31" s="96"/>
     </row>
     <row r="32" spans="3:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="232" t="s">
+      <c r="C32" s="238" t="s">
         <v>207</v>
       </c>
       <c r="D32" s="85" t="s">
@@ -8279,7 +8290,7 @@
       <c r="G32" s="87"/>
     </row>
     <row r="33" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C33" s="233"/>
+      <c r="C33" s="239"/>
       <c r="D33" s="89" t="s">
         <v>180</v>
       </c>
@@ -8290,7 +8301,7 @@
       <c r="G33" s="87"/>
     </row>
     <row r="34" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C34" s="233"/>
+      <c r="C34" s="239"/>
       <c r="D34" s="90" t="s">
         <v>181</v>
       </c>
@@ -8300,7 +8311,7 @@
       <c r="G34" s="88"/>
     </row>
     <row r="35" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C35" s="233"/>
+      <c r="C35" s="239"/>
       <c r="D35" s="90" t="s">
         <v>183</v>
       </c>
@@ -8312,7 +8323,7 @@
       </c>
     </row>
     <row r="36" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C36" s="233"/>
+      <c r="C36" s="239"/>
       <c r="D36" s="91" t="s">
         <v>185</v>
       </c>
@@ -8327,7 +8338,7 @@
       </c>
     </row>
     <row r="37" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C37" s="233"/>
+      <c r="C37" s="239"/>
       <c r="D37" s="94" t="s">
         <v>187</v>
       </c>
@@ -8340,7 +8351,7 @@
       </c>
     </row>
     <row r="38" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C38" s="233"/>
+      <c r="C38" s="239"/>
       <c r="D38" s="89" t="s">
         <v>193</v>
       </c>
@@ -8365,7 +8376,7 @@
       </c>
     </row>
     <row r="39" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C39" s="233"/>
+      <c r="C39" s="239"/>
       <c r="D39" s="90" t="s">
         <v>194</v>
       </c>
@@ -8387,7 +8398,7 @@
       </c>
     </row>
     <row r="40" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C40" s="233"/>
+      <c r="C40" s="239"/>
       <c r="D40" s="90" t="s">
         <v>195</v>
       </c>
@@ -8428,7 +8439,7 @@
       </c>
     </row>
     <row r="41" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C41" s="233"/>
+      <c r="C41" s="239"/>
       <c r="D41" s="91" t="s">
         <v>196</v>
       </c>
@@ -8469,7 +8480,7 @@
       </c>
     </row>
     <row r="42" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C42" s="233"/>
+      <c r="C42" s="239"/>
       <c r="D42" s="80" t="s">
         <v>197</v>
       </c>
@@ -8502,15 +8513,15 @@
       </c>
     </row>
     <row r="43" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C43" s="233"/>
+      <c r="C43" s="239"/>
       <c r="D43" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="E43" s="228" t="s">
+      <c r="E43" s="234" t="s">
         <v>200</v>
       </c>
-      <c r="F43" s="228"/>
-      <c r="G43" s="229"/>
+      <c r="F43" s="234"/>
+      <c r="G43" s="235"/>
       <c r="AA43" s="44">
         <v>13</v>
       </c>
@@ -8539,13 +8550,13 @@
       </c>
     </row>
     <row r="44" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C44" s="234"/>
+      <c r="C44" s="240"/>
       <c r="D44" s="81" t="s">
         <v>199</v>
       </c>
-      <c r="E44" s="230"/>
-      <c r="F44" s="230"/>
-      <c r="G44" s="231"/>
+      <c r="E44" s="236"/>
+      <c r="F44" s="236"/>
+      <c r="G44" s="237"/>
       <c r="AA44" s="44">
         <v>14</v>
       </c>
@@ -8574,7 +8585,7 @@
       </c>
     </row>
     <row r="45" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C45" s="240" t="s">
+      <c r="C45" s="246" t="s">
         <v>216</v>
       </c>
       <c r="D45" s="94" t="s">
@@ -8611,7 +8622,7 @@
       </c>
     </row>
     <row r="46" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C46" s="240"/>
+      <c r="C46" s="246"/>
       <c r="D46" s="89" t="s">
         <v>180</v>
       </c>
@@ -8648,7 +8659,7 @@
       </c>
     </row>
     <row r="47" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C47" s="240"/>
+      <c r="C47" s="246"/>
       <c r="D47" s="90" t="s">
         <v>181</v>
       </c>
@@ -8684,7 +8695,7 @@
       </c>
     </row>
     <row r="48" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C48" s="240"/>
+      <c r="C48" s="246"/>
       <c r="D48" s="90" t="s">
         <v>183</v>
       </c>
@@ -8722,7 +8733,7 @@
       </c>
     </row>
     <row r="49" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C49" s="240"/>
+      <c r="C49" s="246"/>
       <c r="D49" s="90" t="s">
         <v>185</v>
       </c>
@@ -8763,7 +8774,7 @@
       </c>
     </row>
     <row r="50" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C50" s="240"/>
+      <c r="C50" s="246"/>
       <c r="D50" s="93" t="s">
         <v>187</v>
       </c>
@@ -8796,7 +8807,7 @@
       </c>
     </row>
     <row r="51" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C51" s="240"/>
+      <c r="C51" s="246"/>
       <c r="D51" s="90" t="s">
         <v>212</v>
       </c>
@@ -8837,7 +8848,7 @@
       </c>
     </row>
     <row r="52" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C52" s="240"/>
+      <c r="C52" s="246"/>
       <c r="D52" s="93" t="s">
         <v>197</v>
       </c>
@@ -8870,15 +8881,15 @@
       </c>
     </row>
     <row r="53" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C53" s="240"/>
+      <c r="C53" s="246"/>
       <c r="D53" s="90" t="s">
         <v>198</v>
       </c>
-      <c r="E53" s="228" t="s">
+      <c r="E53" s="234" t="s">
         <v>200</v>
       </c>
-      <c r="F53" s="228"/>
-      <c r="G53" s="229"/>
+      <c r="F53" s="234"/>
+      <c r="G53" s="235"/>
       <c r="AA53" s="44">
         <v>23</v>
       </c>
@@ -8907,13 +8918,13 @@
       </c>
     </row>
     <row r="54" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C54" s="240"/>
+      <c r="C54" s="246"/>
       <c r="D54" s="91" t="s">
         <v>199</v>
       </c>
-      <c r="E54" s="230"/>
-      <c r="F54" s="230"/>
-      <c r="G54" s="231"/>
+      <c r="E54" s="236"/>
+      <c r="F54" s="236"/>
+      <c r="G54" s="237"/>
       <c r="AA54" s="44">
         <v>24</v>
       </c>
@@ -8942,7 +8953,7 @@
       </c>
     </row>
     <row r="55" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C55" s="240"/>
+      <c r="C55" s="246"/>
       <c r="D55" s="94" t="s">
         <v>186</v>
       </c>
@@ -8977,7 +8988,7 @@
       </c>
     </row>
     <row r="56" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C56" s="240"/>
+      <c r="C56" s="246"/>
       <c r="D56" s="89" t="s">
         <v>180</v>
       </c>
@@ -9014,7 +9025,7 @@
       </c>
     </row>
     <row r="57" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C57" s="240"/>
+      <c r="C57" s="246"/>
       <c r="D57" s="90" t="s">
         <v>181</v>
       </c>
@@ -9050,7 +9061,7 @@
       </c>
     </row>
     <row r="58" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C58" s="240"/>
+      <c r="C58" s="246"/>
       <c r="D58" s="90" t="s">
         <v>183</v>
       </c>
@@ -9088,7 +9099,7 @@
       </c>
     </row>
     <row r="59" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C59" s="240"/>
+      <c r="C59" s="246"/>
       <c r="D59" s="91" t="s">
         <v>185</v>
       </c>
@@ -9129,7 +9140,7 @@
       </c>
     </row>
     <row r="60" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C60" s="240"/>
+      <c r="C60" s="246"/>
       <c r="D60" s="94" t="s">
         <v>187</v>
       </c>
@@ -9164,7 +9175,7 @@
       </c>
     </row>
     <row r="61" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C61" s="240"/>
+      <c r="C61" s="246"/>
       <c r="D61" s="89" t="s">
         <v>212</v>
       </c>
@@ -9205,7 +9216,7 @@
       </c>
     </row>
     <row r="62" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C62" s="240"/>
+      <c r="C62" s="246"/>
       <c r="D62" s="93" t="s">
         <v>197</v>
       </c>
@@ -9238,15 +9249,15 @@
       </c>
     </row>
     <row r="63" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C63" s="240"/>
+      <c r="C63" s="246"/>
       <c r="D63" s="90" t="s">
         <v>198</v>
       </c>
-      <c r="E63" s="228" t="s">
+      <c r="E63" s="234" t="s">
         <v>200</v>
       </c>
-      <c r="F63" s="228"/>
-      <c r="G63" s="229"/>
+      <c r="F63" s="234"/>
+      <c r="G63" s="235"/>
       <c r="AA63" s="44">
         <v>33</v>
       </c>
@@ -9275,13 +9286,13 @@
       </c>
     </row>
     <row r="64" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C64" s="240"/>
+      <c r="C64" s="246"/>
       <c r="D64" s="91" t="s">
         <v>199</v>
       </c>
-      <c r="E64" s="230"/>
-      <c r="F64" s="230"/>
-      <c r="G64" s="231"/>
+      <c r="E64" s="236"/>
+      <c r="F64" s="236"/>
+      <c r="G64" s="237"/>
       <c r="AA64" s="44">
         <v>34</v>
       </c>
@@ -9433,22 +9444,22 @@
       </c>
     </row>
     <row r="69" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C69" s="232" t="s">
+      <c r="C69" s="238" t="s">
         <v>160</v>
       </c>
-      <c r="D69" s="238" t="s">
+      <c r="D69" s="244" t="s">
         <v>161</v>
       </c>
-      <c r="E69" s="238"/>
-      <c r="F69" s="238" t="s">
+      <c r="E69" s="244"/>
+      <c r="F69" s="244" t="s">
         <v>133</v>
       </c>
-      <c r="G69" s="239"/>
-      <c r="I69" s="235" t="s">
+      <c r="G69" s="245"/>
+      <c r="I69" s="241" t="s">
         <v>223</v>
       </c>
-      <c r="J69" s="236"/>
-      <c r="K69" s="237"/>
+      <c r="J69" s="242"/>
+      <c r="K69" s="243"/>
       <c r="AA69" s="44">
         <v>39</v>
       </c>
@@ -9477,7 +9488,7 @@
       </c>
     </row>
     <row r="70" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C70" s="233"/>
+      <c r="C70" s="239"/>
       <c r="D70" s="15" t="s">
         <v>162</v>
       </c>
@@ -9885,11 +9896,11 @@
         <f t="shared" si="10"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="I77" s="235" t="s">
+      <c r="I77" s="241" t="s">
         <v>222</v>
       </c>
-      <c r="J77" s="236"/>
-      <c r="K77" s="237"/>
+      <c r="J77" s="242"/>
+      <c r="K77" s="243"/>
       <c r="AA77" s="44">
         <v>47</v>
       </c>
@@ -10409,7 +10420,7 @@
       </c>
     </row>
     <row r="90" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C90" s="221" t="s">
+      <c r="C90" s="227" t="s">
         <v>230</v>
       </c>
       <c r="D90" s="86" t="s">
@@ -10462,7 +10473,7 @@
       </c>
     </row>
     <row r="91" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C91" s="222"/>
+      <c r="C91" s="228"/>
       <c r="D91" s="44" t="s">
         <v>232</v>
       </c>
@@ -10513,7 +10524,7 @@
       </c>
     </row>
     <row r="92" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C92" s="222" t="s">
+      <c r="C92" s="228" t="s">
         <v>233</v>
       </c>
       <c r="D92" s="44" t="s">
@@ -10566,7 +10577,7 @@
       </c>
     </row>
     <row r="93" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C93" s="222"/>
+      <c r="C93" s="228"/>
       <c r="D93" s="44" t="s">
         <v>236</v>
       </c>
@@ -10617,7 +10628,7 @@
       </c>
     </row>
     <row r="94" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C94" s="223" t="s">
+      <c r="C94" s="229" t="s">
         <v>234</v>
       </c>
       <c r="D94" s="44" t="s">
@@ -10670,7 +10681,7 @@
       </c>
     </row>
     <row r="95" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C95" s="224"/>
+      <c r="C95" s="230"/>
       <c r="D95" s="81" t="s">
         <v>238</v>
       </c>
@@ -11038,7 +11049,7 @@
       </c>
     </row>
     <row r="126" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C126" s="221" t="s">
+      <c r="C126" s="227" t="s">
         <v>230</v>
       </c>
       <c r="D126" s="86" t="s">
@@ -11065,7 +11076,7 @@
       </c>
     </row>
     <row r="127" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C127" s="222"/>
+      <c r="C127" s="228"/>
       <c r="D127" s="44" t="s">
         <v>232</v>
       </c>
@@ -11090,7 +11101,7 @@
       </c>
     </row>
     <row r="128" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C128" s="222" t="s">
+      <c r="C128" s="228" t="s">
         <v>233</v>
       </c>
       <c r="D128" s="44" t="s">
@@ -11117,7 +11128,7 @@
       </c>
     </row>
     <row r="129" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C129" s="222"/>
+      <c r="C129" s="228"/>
       <c r="D129" s="44" t="s">
         <v>236</v>
       </c>
@@ -11142,7 +11153,7 @@
       </c>
     </row>
     <row r="130" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C130" s="223" t="s">
+      <c r="C130" s="229" t="s">
         <v>234</v>
       </c>
       <c r="D130" s="44" t="s">
@@ -11169,7 +11180,7 @@
       </c>
     </row>
     <row r="131" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C131" s="224"/>
+      <c r="C131" s="230"/>
       <c r="D131" s="81" t="s">
         <v>238</v>
       </c>
@@ -11404,7 +11415,7 @@
       </c>
     </row>
     <row r="163" spans="3:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C163" s="221" t="s">
+      <c r="C163" s="227" t="s">
         <v>230</v>
       </c>
       <c r="D163" s="86" t="s">
@@ -11431,7 +11442,7 @@
       </c>
     </row>
     <row r="164" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C164" s="222"/>
+      <c r="C164" s="228"/>
       <c r="D164" s="44" t="s">
         <v>232</v>
       </c>
@@ -11456,7 +11467,7 @@
       </c>
     </row>
     <row r="165" spans="3:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C165" s="222" t="s">
+      <c r="C165" s="228" t="s">
         <v>233</v>
       </c>
       <c r="D165" s="44" t="s">
@@ -11483,7 +11494,7 @@
       </c>
     </row>
     <row r="166" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C166" s="222"/>
+      <c r="C166" s="228"/>
       <c r="D166" s="44" t="s">
         <v>236</v>
       </c>
@@ -11508,7 +11519,7 @@
       </c>
     </row>
     <row r="167" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C167" s="223" t="s">
+      <c r="C167" s="229" t="s">
         <v>234</v>
       </c>
       <c r="D167" s="44" t="s">
@@ -11535,7 +11546,7 @@
       </c>
     </row>
     <row r="168" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C168" s="224"/>
+      <c r="C168" s="230"/>
       <c r="D168" s="81" t="s">
         <v>238</v>
       </c>
@@ -11789,27 +11800,27 @@
       <c r="L4" s="81"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="235" t="s">
+      <c r="C5" s="241" t="s">
         <v>314</v>
       </c>
-      <c r="D5" s="236"/>
-      <c r="E5" s="236"/>
-      <c r="F5" s="236"/>
-      <c r="G5" s="236"/>
-      <c r="H5" s="237"/>
+      <c r="D5" s="242"/>
+      <c r="E5" s="242"/>
+      <c r="F5" s="242"/>
+      <c r="G5" s="242"/>
+      <c r="H5" s="243"/>
       <c r="I5" s="171" t="s">
         <v>315</v>
       </c>
-      <c r="J5" s="235" t="s">
+      <c r="J5" s="241" t="s">
         <v>316</v>
       </c>
-      <c r="K5" s="236"/>
-      <c r="L5" s="236"/>
-      <c r="M5" s="241" t="s">
+      <c r="K5" s="242"/>
+      <c r="L5" s="242"/>
+      <c r="M5" s="247" t="s">
         <v>322</v>
       </c>
-      <c r="N5" s="238"/>
-      <c r="O5" s="239"/>
+      <c r="N5" s="244"/>
+      <c r="O5" s="245"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C6" s="168" t="s">

</xml_diff>